<commit_message>
added more uct results
</commit_message>
<xml_diff>
--- a/Thesis/MCTS Test Results.xlsx
+++ b/Thesis/MCTS Test Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Guildhall\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B688268-18AC-475E-ADB4-61A4F065EB1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B503577E-732A-42BE-A835-8EAE69F403A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{297119D3-728E-4160-A353-DB4FFAD81E09}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>AI Results</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>7.2 hours</t>
+  </si>
+  <si>
+    <t>MCTS 10k Sarasua 1 UCT sqrt2 vs MCTS 10k Sarasua 1 UCT 0.5</t>
+  </si>
+  <si>
+    <t>10.5/20</t>
+  </si>
+  <si>
+    <t>MCTS 10k Sarasua 1 UCT sqrt2 vs MCTS 10k Sarasua 1 UCT 5</t>
+  </si>
+  <si>
+    <t>11.0/20</t>
   </si>
 </sst>
 </file>
@@ -461,16 +473,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7EA307-2F1F-4558-A660-8CF283252646}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
@@ -572,6 +584,11 @@
         <v>11</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>22</v>
@@ -581,6 +598,30 @@
       </c>
       <c r="D10" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <f>8059/60/60</f>
+        <v>2.2386111111111111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <f>10090/3600</f>
+        <v>2.8027777777777776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added RandomPLUS and updated test results
</commit_message>
<xml_diff>
--- a/Thesis/MCTS Test Results.xlsx
+++ b/Thesis/MCTS Test Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Guildhall\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B503577E-732A-42BE-A835-8EAE69F403A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17896904-CE7C-43B6-88BB-656DA017C672}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{297119D3-728E-4160-A353-DB4FFAD81E09}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>AI Results</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>11.0/20</t>
+  </si>
+  <si>
+    <t>23/50</t>
+  </si>
+  <si>
+    <t>MCTS 10k Sarasua1 0 Chaos vs MCTS Sarasua1 0.15 Chaos</t>
   </si>
 </sst>
 </file>
@@ -473,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7EA307-2F1F-4558-A660-8CF283252646}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,6 +630,18 @@
         <v>2.8027777777777776</v>
       </c>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <f>22684/3600</f>
+        <v>6.3011111111111111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
More data on what next
</commit_message>
<xml_diff>
--- a/Thesis/MCTS Test Results.xlsx
+++ b/Thesis/MCTS Test Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Guildhall\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412E2D3D-368A-44E4-BBFD-B6E50A4BDADB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B09153-C585-49C3-84FE-154B423E50EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{297119D3-728E-4160-A353-DB4FFAD81E09}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>AI Results</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>126/200</t>
+  </si>
+  <si>
+    <t>MCTS 10k Sarasua1 Heuristics 0 Chaos vs 0.05 Chaos</t>
+  </si>
+  <si>
+    <t>18.5/50</t>
   </si>
 </sst>
 </file>
@@ -591,7 +597,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,6 +924,16 @@
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23">
+        <f>15930/3600</f>
+        <v>4.4249999999999998</v>
+      </c>
       <c r="G23" t="s">
         <v>50</v>
       </c>

</xml_diff>